<commit_message>
agregando cosas de promocion inge1
</commit_message>
<xml_diff>
--- a/2do año/Sexto Semestre/ISO/Practicas/p4/ejerciciosAlgoritmos.xlsx
+++ b/2do año/Sexto Semestre/ISO/Practicas/p4/ejerciciosAlgoritmos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\importante\Facultad\2do año\Sexto Semestre\ISO\Practicas\p4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7A449B-E519-4DF5-A5AB-68C1F3C8B9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DED1335-732F-4211-99FE-E28540F3F3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5505" yWindow="2070" windowWidth="20910" windowHeight="11835" xr2:uid="{134E6A5B-724C-4117-B7CA-0DCAE2CEAAA4}"/>
+    <workbookView xWindow="1080" yWindow="3405" windowWidth="20910" windowHeight="11835" xr2:uid="{134E6A5B-724C-4117-B7CA-0DCAE2CEAAA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="62">
   <si>
     <t>Job</t>
   </si>
@@ -217,12 +217,18 @@
   <si>
     <t>(R2,3,2)</t>
   </si>
+  <si>
+    <t>(R2,3,3)</t>
+  </si>
+  <si>
+    <t>(R1,3,2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +255,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -743,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582F71B0-D64A-4387-BE68-73FC70A1C108}">
-  <dimension ref="A4:BI167"/>
+  <dimension ref="A4:BI174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S171" sqref="S171"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J173" sqref="J173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8170,7 +8182,263 @@
         <v>4.666666666666667</v>
       </c>
     </row>
+    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F170" s="3">
+        <v>0</v>
+      </c>
+      <c r="G170" s="3">
+        <v>1</v>
+      </c>
+      <c r="H170" s="3">
+        <v>2</v>
+      </c>
+      <c r="I170" s="3">
+        <v>3</v>
+      </c>
+      <c r="J170" s="3">
+        <v>4</v>
+      </c>
+      <c r="K170" s="3">
+        <v>5</v>
+      </c>
+      <c r="L170" s="3">
+        <v>6</v>
+      </c>
+      <c r="M170" s="3">
+        <v>7</v>
+      </c>
+      <c r="N170" s="3">
+        <v>8</v>
+      </c>
+      <c r="O170" s="3">
+        <v>9</v>
+      </c>
+      <c r="P170" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q170" s="3">
+        <v>11</v>
+      </c>
+      <c r="R170" s="3">
+        <v>12</v>
+      </c>
+      <c r="S170" s="3"/>
+      <c r="T170" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U170" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B171" s="3">
+        <v>1</v>
+      </c>
+      <c r="C171" s="5">
+        <v>1</v>
+      </c>
+      <c r="D171" s="5">
+        <v>3</v>
+      </c>
+      <c r="E171" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F171" s="5"/>
+      <c r="G171" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H171" s="5"/>
+      <c r="I171" s="5">
+        <v>1</v>
+      </c>
+      <c r="J171" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K171" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L171" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M171" s="5"/>
+      <c r="N171" s="5"/>
+      <c r="O171" s="5"/>
+      <c r="P171" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q171" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R171" s="5"/>
+      <c r="S171" s="5"/>
+      <c r="T171" s="5">
+        <v>11</v>
+      </c>
+      <c r="U171" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B172" s="3">
+        <v>2</v>
+      </c>
+      <c r="C172" s="5">
+        <v>0</v>
+      </c>
+      <c r="D172" s="5">
+        <v>6</v>
+      </c>
+      <c r="E172" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G172" s="5">
+        <v>2</v>
+      </c>
+      <c r="H172" s="5">
+        <v>3</v>
+      </c>
+      <c r="I172" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J172" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K172" s="5"/>
+      <c r="L172" s="5"/>
+      <c r="M172" s="5">
+        <v>4</v>
+      </c>
+      <c r="N172" s="5">
+        <v>5</v>
+      </c>
+      <c r="O172" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P172" s="5"/>
+      <c r="Q172" s="5"/>
+      <c r="R172" s="5"/>
+      <c r="S172" s="5"/>
+      <c r="T172" s="5">
+        <v>10</v>
+      </c>
+      <c r="U172" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="3">
+        <v>3</v>
+      </c>
+      <c r="C173" s="5">
+        <v>2</v>
+      </c>
+      <c r="D173" s="5">
+        <v>4</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F173" s="5"/>
+      <c r="G173" s="5"/>
+      <c r="H173" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I173" s="5"/>
+      <c r="J173" s="5">
+        <v>1</v>
+      </c>
+      <c r="K173" s="5">
+        <v>2</v>
+      </c>
+      <c r="L173" s="5">
+        <v>3</v>
+      </c>
+      <c r="M173" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N173" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O173" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P173" s="5"/>
+      <c r="Q173" s="5"/>
+      <c r="R173" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S173" s="5"/>
+      <c r="T173" s="5">
+        <v>11</v>
+      </c>
+      <c r="U173" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B174" s="3"/>
+      <c r="C174" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F174" s="5"/>
+      <c r="G174" s="5"/>
+      <c r="H174" s="5"/>
+      <c r="I174" s="5"/>
+      <c r="J174" s="5"/>
+      <c r="K174" s="5"/>
+      <c r="L174" s="5"/>
+      <c r="M174" s="5"/>
+      <c r="N174" s="5"/>
+      <c r="O174" s="5"/>
+      <c r="P174" s="5"/>
+      <c r="Q174" s="5"/>
+      <c r="R174" s="5"/>
+      <c r="S174" s="5"/>
+      <c r="T174" s="5">
+        <f>AVERAGE(T171:T173)</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="U174" s="5">
+        <f>AVERAGE(U171:U173)</f>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>